<commit_message>
Refatoração Front End - Vagas - Implementando listagem de vagas
</commit_message>
<xml_diff>
--- a/Refatoracao.xlsx
+++ b/Refatoracao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Jean3DSN\tcc\tcc-senai-ds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\backup\Peu\tcc-senai-ds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E1CEB87-DDD7-48AB-89C4-014C0C864318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D96D11-6D3E-44FB-A439-4BBAE4D1D38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8130" windowHeight="2880" xr2:uid="{A3E41196-5843-4D32-9A18-3A37853C1DB1}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11385" xr2:uid="{A3E41196-5843-4D32-9A18-3A37853C1DB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>Cadastrar</t>
   </si>
@@ -143,12 +143,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67555D0B-AA8D-4507-99F0-F0A2AB6CE849}">
   <dimension ref="B3:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,358 +478,360 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="4"/>
+      <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="D24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="4"/>
+      <c r="C29" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="4"/>
+      <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="2"/>
+      <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="4"/>
+      <c r="C39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B18"/>
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refatoração - Cursos - Implementação do cadastro de cursos
</commit_message>
<xml_diff>
--- a/Refatoracao.xlsx
+++ b/Refatoracao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\backup\Peu\tcc-senai-ds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Jean3DSN\tcc\tcc-senai-ds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D96D11-6D3E-44FB-A439-4BBAE4D1D38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F3F352-6EB7-4ACF-BE01-9522A7DC99FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11385" xr2:uid="{A3E41196-5843-4D32-9A18-3A37853C1DB1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
   <si>
     <t>Cadastrar</t>
   </si>
@@ -106,12 +106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -141,12 +147,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67555D0B-AA8D-4507-99F0-F0A2AB6CE849}">
   <dimension ref="B3:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,33 +525,33 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
@@ -588,33 +597,39 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
@@ -650,7 +665,7 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -660,7 +675,7 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,7 +683,7 @@
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="4"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
@@ -676,7 +691,7 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="1" t="s">
         <v>2</v>
       </c>
@@ -748,7 +763,7 @@
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -758,7 +773,7 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +781,7 @@
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="4"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
         <v>1</v>
       </c>
@@ -774,7 +789,7 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="4"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="1" t="s">
         <v>2</v>
       </c>
@@ -784,7 +799,7 @@
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -794,7 +809,7 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="4"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +817,7 @@
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="4"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="1" t="s">
         <v>1</v>
       </c>
@@ -810,7 +825,7 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="4"/>
+      <c r="B39" s="5"/>
       <c r="C39" s="1" t="s">
         <v>2</v>
       </c>
@@ -821,17 +836,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B36:B39"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="B36:B39"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>